<commit_message>
Formatting excel output order sheet
</commit_message>
<xml_diff>
--- a/OUTPUT.xlsx
+++ b/OUTPUT.xlsx
@@ -34,6 +34,9 @@
     <t>YTD 1-Day Momentum Hit Ratio</t>
   </si>
   <si>
+    <t>Order (&gt; 0 =&gt; Buy)</t>
+  </si>
+  <si>
     <t>NVDA</t>
   </si>
   <si>
@@ -92,9 +95,6 @@
   </si>
   <si>
     <t>LYB</t>
-  </si>
-  <si>
-    <t>INCY</t>
   </si>
 </sst>
 </file>
@@ -452,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +477,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -489,10 +492,10 @@
         <v>330</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>198.02</v>
+        <v>204.24</v>
       </c>
       <c r="F2">
         <v>0.01668095238095238</v>
@@ -500,8 +503,11 @@
       <c r="G2">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -512,10 +518,10 @@
         <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>116.73</v>
+        <v>116.96</v>
       </c>
       <c r="F3">
         <v>0.01457619047619048</v>
@@ -523,8 +529,11 @@
       <c r="G3">
         <v>0.7619047619047621</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -535,10 +544,10 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>16.61</v>
+        <v>16.5</v>
       </c>
       <c r="F4">
         <v>0.0138952380952381</v>
@@ -546,8 +555,11 @@
       <c r="G4">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -558,10 +570,10 @@
         <v>291</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>51.78</v>
+        <v>53.58</v>
       </c>
       <c r="F5">
         <v>0.01352857142857143</v>
@@ -569,8 +581,11 @@
       <c r="G5">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -581,10 +596,10 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>262.95</v>
+        <v>266.98</v>
       </c>
       <c r="F6">
         <v>0.01230476190476191</v>
@@ -592,8 +607,11 @@
       <c r="G6">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -604,10 +622,10 @@
         <v>429</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>109.7</v>
+        <v>110.03</v>
       </c>
       <c r="F7">
         <v>0.0115952380952381</v>
@@ -615,8 +633,11 @@
       <c r="G7">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -627,10 +648,10 @@
         <v>203</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8">
-        <v>81.14</v>
+        <v>83.315</v>
       </c>
       <c r="F8">
         <v>0.01061904761904762</v>
@@ -638,8 +659,11 @@
       <c r="G8">
         <v>0.8095238095238098</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -650,10 +674,10 @@
         <v>478</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E9">
-        <v>102.85</v>
+        <v>103.96</v>
       </c>
       <c r="F9">
         <v>0.009771428571428573</v>
@@ -661,8 +685,11 @@
       <c r="G9">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -673,10 +700,10 @@
         <v>396</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10">
-        <v>463.07</v>
+        <v>464.05</v>
       </c>
       <c r="F10">
         <v>0.00969047619047619</v>
@@ -684,8 +711,11 @@
       <c r="G10">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -696,10 +726,10 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>51.32</v>
+        <v>50.86</v>
       </c>
       <c r="F11">
         <v>0.009471428571428572</v>
@@ -707,8 +737,11 @@
       <c r="G11">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -719,10 +752,10 @@
         <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12">
-        <v>2431.15</v>
+        <v>2448.66</v>
       </c>
       <c r="F12">
         <v>0.009466666666666668</v>
@@ -730,8 +763,11 @@
       <c r="G12">
         <v>0.8095238095238098</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -742,10 +778,10 @@
         <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13">
-        <v>72.95</v>
+        <v>73.12</v>
       </c>
       <c r="F13">
         <v>0.0092</v>
@@ -753,8 +789,11 @@
       <c r="G13">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -765,10 +804,10 @@
         <v>450</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14">
-        <v>149.96</v>
+        <v>144.875</v>
       </c>
       <c r="F14">
         <v>0.008419047619047619</v>
@@ -776,8 +815,11 @@
       <c r="G14">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -788,10 +830,10 @@
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15">
-        <v>52.19</v>
+        <v>51.965</v>
       </c>
       <c r="F15">
         <v>0.007804761904761903</v>
@@ -799,8 +841,11 @@
       <c r="G15">
         <v>0.7619047619047621</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -811,10 +856,10 @@
         <v>405</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E16">
-        <v>90.23</v>
+        <v>91.12</v>
       </c>
       <c r="F16">
         <v>0.007595238095238094</v>
@@ -822,8 +867,11 @@
       <c r="G16">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -834,10 +882,10 @@
         <v>435</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17">
-        <v>57.21</v>
+        <v>57.77</v>
       </c>
       <c r="F17">
         <v>0.007485714285714285</v>
@@ -845,8 +893,11 @@
       <c r="G17">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -857,10 +908,10 @@
         <v>415</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18">
-        <v>44.06</v>
+        <v>44.27</v>
       </c>
       <c r="F18">
         <v>0.007057142857142856</v>
@@ -868,8 +919,11 @@
       <c r="G18">
         <v>0.8095238095238098</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -880,10 +934,10 @@
         <v>368</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E19">
-        <v>52.37</v>
+        <v>52.805</v>
       </c>
       <c r="F19">
         <v>0.006395238095238096</v>
@@ -891,8 +945,11 @@
       <c r="G19">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -903,10 +960,10 @@
         <v>434</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E20">
-        <v>710.14</v>
+        <v>706.8200000000001</v>
       </c>
       <c r="F20">
         <v>0.006047619047619046</v>
@@ -914,8 +971,11 @@
       <c r="G20">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -926,10 +986,10 @@
         <v>281</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E21">
-        <v>94.86</v>
+        <v>95.41</v>
       </c>
       <c r="F21">
         <v>0.006042857142857144</v>
@@ -937,28 +997,8 @@
       <c r="G21">
         <v>0.7142857142857144</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>235</v>
-      </c>
-      <c r="C22">
-        <v>235</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22">
-        <v>86.01000000000001</v>
-      </c>
-      <c r="F22">
-        <v>0.003757142857142857</v>
-      </c>
-      <c r="G22">
-        <v>0.7142857142857144</v>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>